<commit_message>
lazy childs problem resolved by doing abortation
</commit_message>
<xml_diff>
--- a/EetdbServices/Docs/example.xlsx
+++ b/EetdbServices/Docs/example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="16650" windowHeight="9390" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="16650" windowHeight="9390"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -281,8 +281,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,8 +456,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -470,9 +470,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -510,7 +510,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -544,6 +544,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -578,9 +579,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -753,232 +755,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="10.5703125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" style="9" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" style="9" customWidth="1"/>
-    <col min="10" max="10" width="36.42578125" style="12" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A2" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="16">
-        <v>0.2</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A3" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="16">
-        <v>0.25</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A4" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="16">
-        <v>0.18</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A5" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="16">
-        <v>0.12</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A6" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="16">
-        <v>0.3</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="F2" r:id="rId6"/>
-    <hyperlink ref="F3" r:id="rId7"/>
-    <hyperlink ref="F4" r:id="rId8"/>
-    <hyperlink ref="F5" r:id="rId9"/>
-    <hyperlink ref="F6" r:id="rId10"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" style="7" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" style="7" customWidth="1"/>
@@ -1001,7 +785,7 @@
     <col min="19" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="13.5" customHeight="1" thickBot="1">
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>86</v>
       </c>
@@ -1057,7 +841,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="3" customFormat="1" ht="13.5" customHeight="1">
+    <row r="2" spans="1:18" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>83</v>
       </c>
@@ -1098,7 +882,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="3" customFormat="1" ht="13.5" customHeight="1">
+    <row r="3" spans="1:18" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>83</v>
       </c>
@@ -1139,7 +923,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="3" customFormat="1" ht="13.5" customHeight="1">
+    <row r="4" spans="1:18" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>84</v>
       </c>
@@ -1196,4 +980,222 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId8"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" style="9" customWidth="1"/>
+    <col min="10" max="10" width="36.42578125" style="12" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="16">
+        <v>0.25</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="16">
+        <v>0.18</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="16">
+        <v>0.12</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="F2" r:id="rId6"/>
+    <hyperlink ref="F3" r:id="rId7"/>
+    <hyperlink ref="F4" r:id="rId8"/>
+    <hyperlink ref="F5" r:id="rId9"/>
+    <hyperlink ref="F6" r:id="rId10"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+</worksheet>
 </file>
</xml_diff>